<commit_message>
Auto commit - 08051742
</commit_message>
<xml_diff>
--- a/IM/202508_Service_Count_Report.xlsx
+++ b/IM/202508_Service_Count_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AA$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AA$56</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="216">
   <si>
     <t>服務次數統計表        篩選月份：202508</t>
   </si>
@@ -448,6 +448,24 @@
     <t>Pm</t>
   </si>
   <si>
+    <t>16:42:00</t>
+  </si>
+  <si>
+    <t>16:57:00</t>
+  </si>
+  <si>
+    <t>T301800012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">台灣大哥大股份有限公司 </t>
+  </si>
+  <si>
+    <t>新北市三重區重新路五段609巷2號2樓</t>
+  </si>
+  <si>
+    <t>台北客服2樓(黑)</t>
+  </si>
+  <si>
     <t>09:48:00</t>
   </si>
   <si>
@@ -505,9 +523,6 @@
     <t>T351500007</t>
   </si>
   <si>
-    <t xml:space="preserve">台灣大哥大股份有限公司 </t>
-  </si>
-  <si>
     <t>新北市三重區重新路五段609巷2號5樓-3(三重湯城維修中</t>
   </si>
   <si>
@@ -520,6 +535,21 @@
     <t>修改設定</t>
   </si>
   <si>
+    <t>16:51:00</t>
+  </si>
+  <si>
+    <t>T351500019</t>
+  </si>
+  <si>
+    <t>新北市三重區重新路五段609巷2號10樓</t>
+  </si>
+  <si>
+    <t>台北客服10樓(彩)</t>
+  </si>
+  <si>
+    <t>黃色攪拌棒偵測器故障</t>
+  </si>
+  <si>
     <t>16:00:00</t>
   </si>
   <si>
@@ -637,7 +667,7 @@
     <t>11:50:00</t>
   </si>
   <si>
-    <t>12:10:00</t>
+    <t>12:13:00</t>
   </si>
   <si>
     <t>THILF04917</t>
@@ -647,13 +677,13 @@
   </si>
   <si>
     <t>板橋翠華店</t>
-  </si>
-  <si>
-    <t>12:13:00</t>
   </si>
   <si>
     <t>錢箱線路換接至TCX800
 測試正常</t>
+  </si>
+  <si>
+    <t>12:10:00</t>
   </si>
   <si>
     <t>12:14:00</t>
@@ -1073,10 +1103,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB53"/>
+  <dimension ref="A1:AB56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1502,7 +1532,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>2025080660</v>
+        <v>2025080659</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
@@ -1541,7 +1571,7 @@
         <v>39</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P7" s="7"/>
       <c r="Q7" s="7">
@@ -1550,7 +1580,9 @@
       <c r="R7" s="7">
         <v>287252</v>
       </c>
-      <c r="S7" s="7"/>
+      <c r="S7" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
@@ -1572,7 +1604,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>2025080659</v>
+        <v>2025080660</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -1611,7 +1643,7 @@
         <v>39</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P8" s="3"/>
       <c r="Q8" s="3">
@@ -1620,9 +1652,7 @@
       <c r="R8" s="3">
         <v>287252</v>
       </c>
-      <c r="S8" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="S8" s="3"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
@@ -2716,7 +2746,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="7">
-        <v>2025080586</v>
+        <v>2025080704</v>
       </c>
       <c r="C25" s="7">
         <v>1</v>
@@ -2755,14 +2785,16 @@
         <v>140</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
       <c r="R25" s="7">
-        <v>163873</v>
-      </c>
-      <c r="S25" s="7"/>
+        <v>7108</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
       <c r="V25" s="7"/>
@@ -2770,21 +2802,17 @@
       <c r="X25" s="7"/>
       <c r="Y25" s="7"/>
       <c r="Z25" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA25" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB25" s="7">
-        <v>1</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7"/>
     </row>
     <row r="26" spans="1:28">
       <c r="A26" s="3">
         <v>24</v>
       </c>
       <c r="B26" s="3">
-        <v>2025080129</v>
+        <v>2025080705</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
@@ -2796,43 +2824,41 @@
         <v>118</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3">
-        <v>253107</v>
-      </c>
-      <c r="S26" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>7108</v>
+      </c>
+      <c r="S26" s="3"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
@@ -2842,7 +2868,9 @@
       <c r="Z26" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="AA26" s="3"/>
+      <c r="AA26" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="AB26" s="3"/>
     </row>
     <row r="27" spans="1:28">
@@ -2850,7 +2878,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="7">
-        <v>2025080130</v>
+        <v>2025080586</v>
       </c>
       <c r="C27" s="7">
         <v>1</v>
@@ -2862,39 +2890,39 @@
         <v>118</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
       <c r="R27" s="7">
-        <v>253107</v>
+        <v>163873</v>
       </c>
       <c r="S27" s="7"/>
       <c r="T27" s="7"/>
@@ -2904,19 +2932,21 @@
       <c r="X27" s="7"/>
       <c r="Y27" s="7"/>
       <c r="Z27" s="8" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="AA27" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AB27" s="7"/>
+      <c r="AB27" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:28">
       <c r="A28" s="3">
         <v>26</v>
       </c>
       <c r="B28" s="3">
-        <v>2025080134</v>
+        <v>2025080129</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
@@ -2931,13 +2961,13 @@
         <v>70</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>47</v>
@@ -2946,13 +2976,13 @@
         <v>36</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="O28" s="3" t="s">
         <v>40</v>
@@ -2960,7 +2990,7 @@
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3">
-        <v>199706</v>
+        <v>253107</v>
       </c>
       <c r="S28" s="3" t="s">
         <v>41</v>
@@ -2982,7 +3012,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="7">
-        <v>2025080135</v>
+        <v>2025080130</v>
       </c>
       <c r="C29" s="7">
         <v>1</v>
@@ -2997,13 +3027,13 @@
         <v>70</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>47</v>
@@ -3012,13 +3042,13 @@
         <v>36</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="M29" s="8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="O29" s="7" t="s">
         <v>43</v>
@@ -3026,7 +3056,7 @@
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
       <c r="R29" s="7">
-        <v>199706</v>
+        <v>253107</v>
       </c>
       <c r="S29" s="7"/>
       <c r="T29" s="7"/>
@@ -3048,7 +3078,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="3">
-        <v>2025080589</v>
+        <v>2025080134</v>
       </c>
       <c r="C30" s="3">
         <v>1</v>
@@ -3060,16 +3090,16 @@
         <v>118</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>47</v>
@@ -3078,13 +3108,13 @@
         <v>36</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>40</v>
@@ -3094,31 +3124,27 @@
       <c r="R30" s="3">
         <v>199706</v>
       </c>
-      <c r="S30" s="3"/>
+      <c r="S30" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="T30" s="3"/>
       <c r="U30" s="3"/>
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
-      <c r="Y30" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="Y30" s="3"/>
       <c r="Z30" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="AA30" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB30" s="3">
-        <v>1</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3"/>
     </row>
     <row r="31" spans="1:28">
       <c r="A31" s="7">
         <v>29</v>
       </c>
       <c r="B31" s="7">
-        <v>2025080415</v>
+        <v>2025080135</v>
       </c>
       <c r="C31" s="7">
         <v>1</v>
@@ -3130,10 +3156,10 @@
         <v>118</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>151</v>
+        <v>85</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>152</v>
@@ -3142,27 +3168,27 @@
         <v>153</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L31" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="M31" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="M31" s="8" t="s">
+      <c r="N31" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="N31" s="8" t="s">
-        <v>156</v>
-      </c>
       <c r="O31" s="7" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
       <c r="R31" s="7">
-        <v>330</v>
+        <v>199706</v>
       </c>
       <c r="S31" s="7"/>
       <c r="T31" s="7"/>
@@ -3172,21 +3198,19 @@
       <c r="X31" s="7"/>
       <c r="Y31" s="7"/>
       <c r="Z31" s="8" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="AA31" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AB31" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB31" s="7"/>
     </row>
     <row r="32" spans="1:28">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" s="3">
-        <v>2025080615</v>
+        <v>2025080589</v>
       </c>
       <c r="C32" s="3">
         <v>1</v>
@@ -3201,36 +3225,36 @@
         <v>31</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>146</v>
+        <v>78</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>153</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L32" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="M32" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="M32" s="6" t="s">
+      <c r="N32" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="N32" s="6" t="s">
-        <v>156</v>
-      </c>
       <c r="O32" s="3" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="3">
-        <v>330</v>
+        <v>199706</v>
       </c>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
@@ -3238,9 +3262,11 @@
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
-      <c r="Y32" s="3"/>
+      <c r="Y32" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="Z32" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AA32" s="3" t="s">
         <v>41</v>
@@ -3254,7 +3280,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="7">
-        <v>2025080143</v>
+        <v>2025080415</v>
       </c>
       <c r="C33" s="7">
         <v>1</v>
@@ -3266,43 +3292,41 @@
         <v>118</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="H33" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="I33" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="I33" s="7" t="s">
-        <v>160</v>
-      </c>
       <c r="J33" s="7" t="s">
-        <v>161</v>
+        <v>54</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
       <c r="R33" s="7">
-        <v>287428</v>
-      </c>
-      <c r="S33" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="S33" s="7"/>
       <c r="T33" s="7"/>
       <c r="U33" s="7"/>
       <c r="V33" s="7"/>
@@ -3310,17 +3334,21 @@
       <c r="X33" s="7"/>
       <c r="Y33" s="7"/>
       <c r="Z33" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA33" s="7"/>
-      <c r="AB33" s="7"/>
+        <v>162</v>
+      </c>
+      <c r="AA33" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB33" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:28">
       <c r="A34" s="3">
         <v>32</v>
       </c>
       <c r="B34" s="3">
-        <v>2025080144</v>
+        <v>2025080615</v>
       </c>
       <c r="C34" s="3">
         <v>1</v>
@@ -3332,39 +3360,39 @@
         <v>118</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="H34" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I34" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I34" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="J34" s="3" t="s">
-        <v>161</v>
+        <v>54</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3">
-        <v>287428</v>
+        <v>330</v>
       </c>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
@@ -3374,19 +3402,21 @@
       <c r="X34" s="3"/>
       <c r="Y34" s="3"/>
       <c r="Z34" s="6" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="AA34" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AB34" s="3"/>
+      <c r="AB34" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:28">
       <c r="A35" s="7">
         <v>33</v>
       </c>
       <c r="B35" s="7">
-        <v>2025080132</v>
+        <v>2025080696</v>
       </c>
       <c r="C35" s="7">
         <v>1</v>
@@ -3398,25 +3428,25 @@
         <v>118</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>85</v>
+        <v>164</v>
       </c>
       <c r="I35" s="7" t="s">
         <v>165</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>161</v>
+        <v>54</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="M35" s="8" t="s">
         <v>166</v>
@@ -3425,16 +3455,16 @@
         <v>167</v>
       </c>
       <c r="O35" s="7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="P35" s="7"/>
-      <c r="Q35" s="7"/>
+      <c r="Q35" s="7">
+        <v>6663</v>
+      </c>
       <c r="R35" s="7">
-        <v>116181</v>
-      </c>
-      <c r="S35" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>11174</v>
+      </c>
+      <c r="S35" s="7"/>
       <c r="T35" s="7"/>
       <c r="U35" s="7"/>
       <c r="V35" s="7"/>
@@ -3442,17 +3472,21 @@
       <c r="X35" s="7"/>
       <c r="Y35" s="7"/>
       <c r="Z35" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA35" s="7"/>
-      <c r="AB35" s="7"/>
+        <v>168</v>
+      </c>
+      <c r="AA35" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB35" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:28">
       <c r="A36" s="3">
         <v>34</v>
       </c>
       <c r="B36" s="3">
-        <v>2025080133</v>
+        <v>2025080143</v>
       </c>
       <c r="C36" s="3">
         <v>1</v>
@@ -3467,38 +3501,40 @@
         <v>70</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>85</v>
+        <v>169</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="K36" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="M36" s="6" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3">
-        <v>116181</v>
-      </c>
-      <c r="S36" s="3"/>
+        <v>287428</v>
+      </c>
+      <c r="S36" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
@@ -3508,9 +3544,7 @@
       <c r="Z36" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="AA36" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA36" s="3"/>
       <c r="AB36" s="3"/>
     </row>
     <row r="37" spans="1:28">
@@ -3518,7 +3552,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="7">
-        <v>2025080027</v>
+        <v>2025080144</v>
       </c>
       <c r="C37" s="7">
         <v>1</v>
@@ -3533,40 +3567,38 @@
         <v>70</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>77</v>
+        <v>169</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="M37" s="8" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="N37" s="8" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="O37" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
       <c r="R37" s="7">
-        <v>180622</v>
-      </c>
-      <c r="S37" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>287428</v>
+      </c>
+      <c r="S37" s="7"/>
       <c r="T37" s="7"/>
       <c r="U37" s="7"/>
       <c r="V37" s="7"/>
@@ -3576,7 +3608,9 @@
       <c r="Z37" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="AA37" s="7"/>
+      <c r="AA37" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="AB37" s="7"/>
     </row>
     <row r="38" spans="1:28">
@@ -3584,7 +3618,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="3">
-        <v>2025080028</v>
+        <v>2025080132</v>
       </c>
       <c r="C38" s="3">
         <v>1</v>
@@ -3599,38 +3633,40 @@
         <v>70</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>168</v>
+        <v>128</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="K38" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
       <c r="R38" s="3">
-        <v>180622</v>
-      </c>
-      <c r="S38" s="3"/>
+        <v>116181</v>
+      </c>
+      <c r="S38" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="T38" s="3"/>
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
@@ -3640,9 +3676,7 @@
       <c r="Z38" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="AA38" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA38" s="3"/>
       <c r="AB38" s="3"/>
     </row>
     <row r="39" spans="1:28">
@@ -3650,7 +3684,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="7">
-        <v>2025080029</v>
+        <v>2025080133</v>
       </c>
       <c r="C39" s="7">
         <v>1</v>
@@ -3665,36 +3699,36 @@
         <v>70</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="H39" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="J39" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="J39" s="7" t="s">
-        <v>161</v>
       </c>
       <c r="K39" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="M39" s="8" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="N39" s="8" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="O39" s="7" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
       <c r="R39" s="7">
-        <v>180622</v>
+        <v>116181</v>
       </c>
       <c r="S39" s="7"/>
       <c r="T39" s="7"/>
@@ -3704,7 +3738,7 @@
       <c r="X39" s="7"/>
       <c r="Y39" s="7"/>
       <c r="Z39" s="8" t="s">
-        <v>172</v>
+        <v>134</v>
       </c>
       <c r="AA39" s="7" t="s">
         <v>41</v>
@@ -3716,7 +3750,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="3">
-        <v>2025080588</v>
+        <v>2025080027</v>
       </c>
       <c r="C40" s="3">
         <v>1</v>
@@ -3728,31 +3762,31 @@
         <v>118</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>77</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="O40" s="3" t="s">
         <v>40</v>
@@ -3762,31 +3796,27 @@
       <c r="R40" s="3">
         <v>180622</v>
       </c>
-      <c r="S40" s="3"/>
+      <c r="S40" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
       <c r="X40" s="3"/>
-      <c r="Y40" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="Y40" s="3"/>
       <c r="Z40" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="AA40" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB40" s="3">
-        <v>1</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="AA40" s="3"/>
+      <c r="AB40" s="3"/>
     </row>
     <row r="41" spans="1:28">
       <c r="A41" s="7">
         <v>39</v>
       </c>
       <c r="B41" s="7">
-        <v>2025080136</v>
+        <v>2025080028</v>
       </c>
       <c r="C41" s="7">
         <v>1</v>
@@ -3801,40 +3831,38 @@
         <v>70</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="K41" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="M41" s="8" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="N41" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="O41" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="7">
-        <v>342829</v>
-      </c>
-      <c r="S41" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>180622</v>
+      </c>
+      <c r="S41" s="7"/>
       <c r="T41" s="7"/>
       <c r="U41" s="7"/>
       <c r="V41" s="7"/>
@@ -3844,7 +3872,9 @@
       <c r="Z41" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="AA41" s="7"/>
+      <c r="AA41" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="AB41" s="7"/>
     </row>
     <row r="42" spans="1:28">
@@ -3852,7 +3882,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="3">
-        <v>2025080137</v>
+        <v>2025080029</v>
       </c>
       <c r="C42" s="3">
         <v>1</v>
@@ -3867,36 +3897,36 @@
         <v>70</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>146</v>
+        <v>77</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="K42" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="M42" s="6" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
       <c r="R42" s="3">
-        <v>342829</v>
+        <v>180622</v>
       </c>
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
@@ -3906,7 +3936,7 @@
       <c r="X42" s="3"/>
       <c r="Y42" s="3"/>
       <c r="Z42" s="6" t="s">
-        <v>134</v>
+        <v>182</v>
       </c>
       <c r="AA42" s="3" t="s">
         <v>41</v>
@@ -3918,7 +3948,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="7">
-        <v>2025080642</v>
+        <v>2025080588</v>
       </c>
       <c r="C43" s="7">
         <v>1</v>
@@ -3933,28 +3963,28 @@
         <v>31</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="K43" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="M43" s="8" t="s">
         <v>180</v>
       </c>
       <c r="N43" s="8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="O43" s="7" t="s">
         <v>40</v>
@@ -3962,29 +3992,33 @@
       <c r="P43" s="7"/>
       <c r="Q43" s="7"/>
       <c r="R43" s="7">
-        <v>31483</v>
-      </c>
-      <c r="S43" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>180622</v>
+      </c>
+      <c r="S43" s="7"/>
       <c r="T43" s="7"/>
       <c r="U43" s="7"/>
       <c r="V43" s="7"/>
       <c r="W43" s="7"/>
       <c r="X43" s="7"/>
-      <c r="Y43" s="7"/>
+      <c r="Y43" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="Z43" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA43" s="7"/>
-      <c r="AB43" s="7"/>
+        <v>183</v>
+      </c>
+      <c r="AA43" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB43" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:28">
       <c r="A44" s="3">
         <v>42</v>
       </c>
       <c r="B44" s="3">
-        <v>2025080643</v>
+        <v>2025080137</v>
       </c>
       <c r="C44" s="3">
         <v>1</v>
@@ -3996,31 +4030,31 @@
         <v>118</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="K44" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="M44" s="6" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="N44" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="O44" s="3" t="s">
         <v>43</v>
@@ -4028,7 +4062,7 @@
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
       <c r="R44" s="3">
-        <v>31483</v>
+        <v>342829</v>
       </c>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
@@ -4043,14 +4077,16 @@
       <c r="AA44" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AB44" s="3"/>
+      <c r="AB44" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:28">
       <c r="A45" s="7">
         <v>43</v>
       </c>
       <c r="B45" s="7">
-        <v>2025080447</v>
+        <v>2025080136</v>
       </c>
       <c r="C45" s="7">
         <v>1</v>
@@ -4062,27 +4098,31 @@
         <v>118</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
+        <v>184</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="L45" s="8" t="s">
-        <v>63</v>
+        <v>149</v>
       </c>
       <c r="M45" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="N45" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="O45" s="7" t="s">
         <v>40</v>
@@ -4090,7 +4130,7 @@
       <c r="P45" s="7"/>
       <c r="Q45" s="7"/>
       <c r="R45" s="7">
-        <v>0</v>
+        <v>342829</v>
       </c>
       <c r="S45" s="7" t="s">
         <v>41</v>
@@ -4102,21 +4142,17 @@
       <c r="X45" s="7"/>
       <c r="Y45" s="7"/>
       <c r="Z45" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA45" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB45" s="7">
-        <v>1</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="AA45" s="7"/>
+      <c r="AB45" s="7"/>
     </row>
     <row r="46" spans="1:28">
       <c r="A46" s="3">
         <v>44</v>
       </c>
       <c r="B46" s="3">
-        <v>2025080035</v>
+        <v>2025080642</v>
       </c>
       <c r="C46" s="3">
         <v>1</v>
@@ -4128,41 +4164,43 @@
         <v>118</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>187</v>
+        <v>127</v>
       </c>
       <c r="I46" s="3" t="s">
         <v>188</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>61</v>
+        <v>189</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>63</v>
+        <v>131</v>
       </c>
       <c r="M46" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
       <c r="R46" s="3">
-        <v>0</v>
-      </c>
-      <c r="S46" s="3"/>
+        <v>31483</v>
+      </c>
+      <c r="S46" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="T46" s="3"/>
       <c r="U46" s="3"/>
       <c r="V46" s="3"/>
@@ -4170,21 +4208,17 @@
       <c r="X46" s="3"/>
       <c r="Y46" s="3"/>
       <c r="Z46" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="AA46" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB46" s="3">
-        <v>1</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="AA46" s="3"/>
+      <c r="AB46" s="3"/>
     </row>
     <row r="47" spans="1:28">
       <c r="A47" s="7">
         <v>45</v>
       </c>
       <c r="B47" s="7">
-        <v>2025080425</v>
+        <v>2025080643</v>
       </c>
       <c r="C47" s="7">
         <v>1</v>
@@ -4196,39 +4230,41 @@
         <v>118</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>77</v>
+        <v>127</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
+        <v>188</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="K47" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="L47" s="8" t="s">
-        <v>63</v>
+        <v>131</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="O47" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P47" s="7"/>
       <c r="Q47" s="7"/>
       <c r="R47" s="7">
-        <v>0</v>
-      </c>
-      <c r="S47" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>31483</v>
+      </c>
+      <c r="S47" s="7"/>
       <c r="T47" s="7"/>
       <c r="U47" s="7"/>
       <c r="V47" s="7"/>
@@ -4236,21 +4272,19 @@
       <c r="X47" s="7"/>
       <c r="Y47" s="7"/>
       <c r="Z47" s="8" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="AA47" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AB47" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB47" s="7"/>
     </row>
     <row r="48" spans="1:28">
       <c r="A48" s="3">
         <v>46</v>
       </c>
       <c r="B48" s="3">
-        <v>2025080426</v>
+        <v>2025080447</v>
       </c>
       <c r="C48" s="3">
         <v>1</v>
@@ -4265,13 +4299,13 @@
         <v>57</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>168</v>
+        <v>113</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>77</v>
+        <v>192</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -4279,10 +4313,10 @@
         <v>63</v>
       </c>
       <c r="M48" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O48" s="3" t="s">
         <v>40</v>
@@ -4307,14 +4341,16 @@
       <c r="AA48" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AB48" s="3"/>
+      <c r="AB48" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="1:28">
       <c r="A49" s="7">
         <v>47</v>
       </c>
       <c r="B49" s="7">
-        <v>2025080367</v>
+        <v>2025080035</v>
       </c>
       <c r="C49" s="7">
         <v>1</v>
@@ -4326,16 +4362,16 @@
         <v>118</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="J49" s="7" t="s">
         <v>61</v>
@@ -4347,10 +4383,10 @@
         <v>63</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="N49" s="8" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="O49" s="7" t="s">
         <v>66</v>
@@ -4368,19 +4404,21 @@
       <c r="X49" s="7"/>
       <c r="Y49" s="7"/>
       <c r="Z49" s="8" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="AA49" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AB49" s="7"/>
+      <c r="AB49" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:28">
       <c r="A50" s="3">
         <v>48</v>
       </c>
       <c r="B50" s="3">
-        <v>2025080636</v>
+        <v>2025080425</v>
       </c>
       <c r="C50" s="3">
         <v>1</v>
@@ -4389,19 +4427,19 @@
         <v>29</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>196</v>
+        <v>118</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>198</v>
+        <v>77</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -4409,10 +4447,10 @@
         <v>63</v>
       </c>
       <c r="M50" s="6" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="N50" s="6" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="O50" s="3" t="s">
         <v>40</v>
@@ -4446,7 +4484,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="7">
-        <v>2025080521</v>
+        <v>2025080426</v>
       </c>
       <c r="C51" s="7">
         <v>1</v>
@@ -4455,44 +4493,42 @@
         <v>29</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>196</v>
+        <v>118</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="H51" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I51" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="I51" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="J51" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="K51" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
       <c r="L51" s="8" t="s">
         <v>63</v>
       </c>
       <c r="M51" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="N51" s="8" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="O51" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="P51" s="7"/>
       <c r="Q51" s="7"/>
       <c r="R51" s="7">
         <v>0</v>
       </c>
-      <c r="S51" s="7"/>
+      <c r="S51" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="T51" s="7"/>
       <c r="U51" s="7"/>
       <c r="V51" s="7"/>
@@ -4500,7 +4536,7 @@
       <c r="X51" s="7"/>
       <c r="Y51" s="7"/>
       <c r="Z51" s="8" t="s">
-        <v>203</v>
+        <v>76</v>
       </c>
       <c r="AA51" s="7" t="s">
         <v>41</v>
@@ -4512,7 +4548,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="3">
-        <v>2025080527</v>
+        <v>2025080367</v>
       </c>
       <c r="C52" s="3">
         <v>1</v>
@@ -4521,19 +4557,19 @@
         <v>29</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>196</v>
+        <v>118</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>197</v>
+        <v>77</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>61</v>
@@ -4545,10 +4581,10 @@
         <v>63</v>
       </c>
       <c r="M52" s="6" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="O52" s="3" t="s">
         <v>66</v>
@@ -4566,7 +4602,7 @@
       <c r="X52" s="3"/>
       <c r="Y52" s="3"/>
       <c r="Z52" s="6" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AA52" s="3" t="s">
         <v>41</v>
@@ -4574,37 +4610,235 @@
       <c r="AB52" s="3"/>
     </row>
     <row r="53" spans="1:28">
-      <c r="A53" s="9"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
-      <c r="K53" s="9"/>
-      <c r="L53" s="10"/>
-      <c r="M53" s="10"/>
-      <c r="N53" s="10"/>
-      <c r="O53" s="9"/>
-      <c r="P53" s="9"/>
-      <c r="Q53" s="9"/>
-      <c r="R53" s="9"/>
-      <c r="S53" s="9"/>
-      <c r="T53" s="9"/>
-      <c r="U53" s="9"/>
-      <c r="V53" s="9"/>
-      <c r="W53" s="9"/>
-      <c r="X53" s="9"/>
-      <c r="Y53" s="9"/>
-      <c r="Z53" s="10"/>
-      <c r="AA53" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="AB53" s="9">
-        <v>22</v>
+      <c r="A53" s="7">
+        <v>51</v>
+      </c>
+      <c r="B53" s="7">
+        <v>2025080521</v>
+      </c>
+      <c r="C53" s="7">
+        <v>1</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="J53" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K53" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L53" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="M53" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="N53" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="O53" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P53" s="7"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="7">
+        <v>0</v>
+      </c>
+      <c r="S53" s="7"/>
+      <c r="T53" s="7"/>
+      <c r="U53" s="7"/>
+      <c r="V53" s="7"/>
+      <c r="W53" s="7"/>
+      <c r="X53" s="7"/>
+      <c r="Y53" s="7"/>
+      <c r="Z53" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="AA53" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB53" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28">
+      <c r="A54" s="3">
+        <v>52</v>
+      </c>
+      <c r="B54" s="3">
+        <v>2025080636</v>
+      </c>
+      <c r="C54" s="3">
+        <v>1</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M54" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="N54" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="O54" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3"/>
+      <c r="R54" s="3">
+        <v>0</v>
+      </c>
+      <c r="S54" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T54" s="3"/>
+      <c r="U54" s="3"/>
+      <c r="V54" s="3"/>
+      <c r="W54" s="3"/>
+      <c r="X54" s="3"/>
+      <c r="Y54" s="3"/>
+      <c r="Z54" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA54" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB54" s="3"/>
+    </row>
+    <row r="55" spans="1:28">
+      <c r="A55" s="7">
+        <v>53</v>
+      </c>
+      <c r="B55" s="7">
+        <v>2025080527</v>
+      </c>
+      <c r="C55" s="7">
+        <v>1</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L55" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="M55" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="N55" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="O55" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="7">
+        <v>0</v>
+      </c>
+      <c r="S55" s="7"/>
+      <c r="T55" s="7"/>
+      <c r="U55" s="7"/>
+      <c r="V55" s="7"/>
+      <c r="W55" s="7"/>
+      <c r="X55" s="7"/>
+      <c r="Y55" s="7"/>
+      <c r="Z55" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="AA55" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB55" s="7"/>
+    </row>
+    <row r="56" spans="1:28">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="10"/>
+      <c r="M56" s="10"/>
+      <c r="N56" s="10"/>
+      <c r="O56" s="9"/>
+      <c r="P56" s="9"/>
+      <c r="Q56" s="9"/>
+      <c r="R56" s="9"/>
+      <c r="S56" s="9"/>
+      <c r="T56" s="9"/>
+      <c r="U56" s="9"/>
+      <c r="V56" s="9"/>
+      <c r="W56" s="9"/>
+      <c r="X56" s="9"/>
+      <c r="Y56" s="9"/>
+      <c r="Z56" s="10"/>
+      <c r="AA56" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB56" s="9">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit - 08061227
</commit_message>
<xml_diff>
--- a/IM/202508_Service_Count_Report.xlsx
+++ b/IM/202508_Service_Count_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AA$56</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AA$58</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="227">
   <si>
     <t>服務次數統計表        篩選月份：202508</t>
   </si>
@@ -535,6 +535,30 @@
     <t>修改設定</t>
   </si>
   <si>
+    <t>2025-08-06</t>
+  </si>
+  <si>
+    <t>10:30:00</t>
+  </si>
+  <si>
+    <t>11:50:00</t>
+  </si>
+  <si>
+    <t>T351500013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">台灣固網股份有限公司 </t>
+  </si>
+  <si>
+    <t>新北市三重區重新路5段609巷2號4F(三重湯城)</t>
+  </si>
+  <si>
+    <t>三重湯城4樓(固網客服)(彩)</t>
+  </si>
+  <si>
+    <t>整機 取送分輪 radf分輪</t>
+  </si>
+  <si>
     <t>16:51:00</t>
   </si>
   <si>
@@ -586,9 +610,6 @@
     <t>新北市五股區五工六路35號4樓(五股)</t>
   </si>
   <si>
-    <t>10:30:00</t>
-  </si>
-  <si>
     <t>黑線髒污 更換OD OD刮 回刮</t>
   </si>
   <si>
@@ -604,6 +625,21 @@
     <t>五股檢品</t>
   </si>
   <si>
+    <t>T451800007</t>
+  </si>
+  <si>
+    <t>eS-4518A 黑白複合機</t>
+  </si>
+  <si>
+    <t>新北市三重區重新路五段609巷2號10樓-3</t>
+  </si>
+  <si>
+    <t>台北客服10樓-3(黑)</t>
+  </si>
+  <si>
+    <t>更換上熱 分爪 OD OD刮 回刮</t>
+  </si>
+  <si>
     <t>13:00:00</t>
   </si>
   <si>
@@ -664,26 +700,23 @@
     <t>狄澤洋</t>
   </si>
   <si>
-    <t>11:50:00</t>
+    <t>12:10:00</t>
+  </si>
+  <si>
+    <t>THILF04917</t>
+  </si>
+  <si>
+    <t>新北市板橋區翠華街6巷1號1樓</t>
+  </si>
+  <si>
+    <t>板橋翠華店</t>
   </si>
   <si>
     <t>12:13:00</t>
-  </si>
-  <si>
-    <t>THILF04917</t>
-  </si>
-  <si>
-    <t>新北市板橋區翠華街6巷1號1樓</t>
-  </si>
-  <si>
-    <t>板橋翠華店</t>
   </si>
   <si>
     <t>錢箱線路換接至TCX800
 測試正常</t>
-  </si>
-  <si>
-    <t>12:10:00</t>
   </si>
   <si>
     <t>12:14:00</t>
@@ -1103,10 +1136,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB56"/>
+  <dimension ref="A1:AB58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3416,7 +3449,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="7">
-        <v>2025080696</v>
+        <v>2025080775</v>
       </c>
       <c r="C35" s="7">
         <v>1</v>
@@ -3428,16 +3461,16 @@
         <v>118</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>31</v>
+        <v>164</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="J35" s="7" t="s">
         <v>54</v>
@@ -3446,23 +3479,23 @@
         <v>36</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="M35" s="8" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N35" s="8" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="O35" s="7" t="s">
         <v>66</v>
       </c>
       <c r="P35" s="7"/>
       <c r="Q35" s="7">
-        <v>6663</v>
+        <v>1595</v>
       </c>
       <c r="R35" s="7">
-        <v>11174</v>
+        <v>27090</v>
       </c>
       <c r="S35" s="7"/>
       <c r="T35" s="7"/>
@@ -3472,7 +3505,7 @@
       <c r="X35" s="7"/>
       <c r="Y35" s="7"/>
       <c r="Z35" s="8" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="AA35" s="7" t="s">
         <v>41</v>
@@ -3486,7 +3519,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="3">
-        <v>2025080143</v>
+        <v>2025080696</v>
       </c>
       <c r="C36" s="3">
         <v>1</v>
@@ -3498,43 +3531,43 @@
         <v>118</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>157</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>171</v>
+        <v>54</v>
       </c>
       <c r="K36" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="M36" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
+      <c r="Q36" s="3">
+        <v>6663</v>
+      </c>
       <c r="R36" s="3">
-        <v>287428</v>
-      </c>
-      <c r="S36" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>11174</v>
+      </c>
+      <c r="S36" s="3"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
@@ -3542,17 +3575,21 @@
       <c r="X36" s="3"/>
       <c r="Y36" s="3"/>
       <c r="Z36" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA36" s="3"/>
-      <c r="AB36" s="3"/>
+        <v>176</v>
+      </c>
+      <c r="AA36" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB36" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:28">
       <c r="A37" s="7">
         <v>35</v>
       </c>
       <c r="B37" s="7">
-        <v>2025080144</v>
+        <v>2025080143</v>
       </c>
       <c r="C37" s="7">
         <v>1</v>
@@ -3570,35 +3607,37 @@
         <v>157</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="M37" s="8" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="N37" s="8" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="O37" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
       <c r="R37" s="7">
         <v>287428</v>
       </c>
-      <c r="S37" s="7"/>
+      <c r="S37" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="T37" s="7"/>
       <c r="U37" s="7"/>
       <c r="V37" s="7"/>
@@ -3608,9 +3647,7 @@
       <c r="Z37" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="AA37" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA37" s="7"/>
       <c r="AB37" s="7"/>
     </row>
     <row r="38" spans="1:28">
@@ -3618,7 +3655,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="3">
-        <v>2025080132</v>
+        <v>2025080144</v>
       </c>
       <c r="C38" s="3">
         <v>1</v>
@@ -3633,40 +3670,38 @@
         <v>70</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>85</v>
+        <v>177</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="K38" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>149</v>
+        <v>180</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
       <c r="R38" s="3">
-        <v>116181</v>
-      </c>
-      <c r="S38" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>287428</v>
+      </c>
+      <c r="S38" s="3"/>
       <c r="T38" s="3"/>
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
@@ -3676,7 +3711,9 @@
       <c r="Z38" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="AA38" s="3"/>
+      <c r="AA38" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="AB38" s="3"/>
     </row>
     <row r="39" spans="1:28">
@@ -3684,7 +3721,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="7">
-        <v>2025080133</v>
+        <v>2025080132</v>
       </c>
       <c r="C39" s="7">
         <v>1</v>
@@ -3705,10 +3742,10 @@
         <v>85</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="K39" s="7" t="s">
         <v>36</v>
@@ -3717,20 +3754,22 @@
         <v>149</v>
       </c>
       <c r="M39" s="8" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="N39" s="8" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="O39" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
       <c r="R39" s="7">
         <v>116181</v>
       </c>
-      <c r="S39" s="7"/>
+      <c r="S39" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="T39" s="7"/>
       <c r="U39" s="7"/>
       <c r="V39" s="7"/>
@@ -3740,9 +3779,7 @@
       <c r="Z39" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="AA39" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA39" s="7"/>
       <c r="AB39" s="7"/>
     </row>
     <row r="40" spans="1:28">
@@ -3750,7 +3787,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="3">
-        <v>2025080027</v>
+        <v>2025080133</v>
       </c>
       <c r="C40" s="3">
         <v>1</v>
@@ -3765,16 +3802,16 @@
         <v>70</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I40" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="J40" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>36</v>
@@ -3783,22 +3820,20 @@
         <v>149</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3">
-        <v>180622</v>
-      </c>
-      <c r="S40" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>116181</v>
+      </c>
+      <c r="S40" s="3"/>
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
@@ -3808,7 +3843,9 @@
       <c r="Z40" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="AA40" s="3"/>
+      <c r="AA40" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="AB40" s="3"/>
     </row>
     <row r="41" spans="1:28">
@@ -3816,7 +3853,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="7">
-        <v>2025080028</v>
+        <v>2025080027</v>
       </c>
       <c r="C41" s="7">
         <v>1</v>
@@ -3831,16 +3868,16 @@
         <v>70</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>77</v>
       </c>
       <c r="I41" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="J41" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>171</v>
       </c>
       <c r="K41" s="7" t="s">
         <v>36</v>
@@ -3849,20 +3886,22 @@
         <v>149</v>
       </c>
       <c r="M41" s="8" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="N41" s="8" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="O41" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="7">
         <v>180622</v>
       </c>
-      <c r="S41" s="7"/>
+      <c r="S41" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="T41" s="7"/>
       <c r="U41" s="7"/>
       <c r="V41" s="7"/>
@@ -3872,9 +3911,7 @@
       <c r="Z41" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="AA41" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA41" s="7"/>
       <c r="AB41" s="7"/>
     </row>
     <row r="42" spans="1:28">
@@ -3882,7 +3919,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="3">
-        <v>2025080029</v>
+        <v>2025080028</v>
       </c>
       <c r="C42" s="3">
         <v>1</v>
@@ -3897,16 +3934,16 @@
         <v>70</v>
       </c>
       <c r="G42" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H42" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H42" s="3" t="s">
-        <v>181</v>
-      </c>
       <c r="I42" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J42" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="K42" s="3" t="s">
         <v>36</v>
@@ -3915,13 +3952,13 @@
         <v>149</v>
       </c>
       <c r="M42" s="6" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
@@ -3936,7 +3973,7 @@
       <c r="X42" s="3"/>
       <c r="Y42" s="3"/>
       <c r="Z42" s="6" t="s">
-        <v>182</v>
+        <v>134</v>
       </c>
       <c r="AA42" s="3" t="s">
         <v>41</v>
@@ -3948,7 +3985,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="7">
-        <v>2025080588</v>
+        <v>2025080029</v>
       </c>
       <c r="C43" s="7">
         <v>1</v>
@@ -3960,19 +3997,19 @@
         <v>118</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>178</v>
+        <v>77</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="I43" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="J43" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>171</v>
       </c>
       <c r="K43" s="7" t="s">
         <v>36</v>
@@ -3981,13 +4018,13 @@
         <v>149</v>
       </c>
       <c r="M43" s="8" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="N43" s="8" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="O43" s="7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="P43" s="7"/>
       <c r="Q43" s="7"/>
@@ -4000,25 +4037,21 @@
       <c r="V43" s="7"/>
       <c r="W43" s="7"/>
       <c r="X43" s="7"/>
-      <c r="Y43" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="Y43" s="7"/>
       <c r="Z43" s="8" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="AA43" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AB43" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB43" s="7"/>
     </row>
     <row r="44" spans="1:28">
       <c r="A44" s="3">
         <v>42</v>
       </c>
       <c r="B44" s="3">
-        <v>2025080137</v>
+        <v>2025080588</v>
       </c>
       <c r="C44" s="3">
         <v>1</v>
@@ -4030,19 +4063,19 @@
         <v>118</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>152</v>
+        <v>186</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>157</v>
+        <v>77</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="K44" s="3" t="s">
         <v>36</v>
@@ -4051,18 +4084,18 @@
         <v>149</v>
       </c>
       <c r="M44" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="N44" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="N44" s="6" t="s">
-        <v>186</v>
-      </c>
       <c r="O44" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
       <c r="R44" s="3">
-        <v>342829</v>
+        <v>180622</v>
       </c>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
@@ -4070,9 +4103,11 @@
       <c r="V44" s="3"/>
       <c r="W44" s="3"/>
       <c r="X44" s="3"/>
-      <c r="Y44" s="3"/>
+      <c r="Y44" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="Z44" s="6" t="s">
-        <v>134</v>
+        <v>190</v>
       </c>
       <c r="AA44" s="3" t="s">
         <v>41</v>
@@ -4107,10 +4142,10 @@
         <v>157</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="K45" s="7" t="s">
         <v>36</v>
@@ -4119,10 +4154,10 @@
         <v>149</v>
       </c>
       <c r="M45" s="8" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="N45" s="8" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="O45" s="7" t="s">
         <v>40</v>
@@ -4152,7 +4187,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="3">
-        <v>2025080642</v>
+        <v>2025080137</v>
       </c>
       <c r="C46" s="3">
         <v>1</v>
@@ -4164,43 +4199,41 @@
         <v>118</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="K46" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="M46" s="6" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
       <c r="R46" s="3">
-        <v>31483</v>
-      </c>
-      <c r="S46" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>342829</v>
+      </c>
+      <c r="S46" s="3"/>
       <c r="T46" s="3"/>
       <c r="U46" s="3"/>
       <c r="V46" s="3"/>
@@ -4210,7 +4243,9 @@
       <c r="Z46" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="AA46" s="3"/>
+      <c r="AA46" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="AB46" s="3"/>
     </row>
     <row r="47" spans="1:28">
@@ -4218,7 +4253,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="7">
-        <v>2025080643</v>
+        <v>2025080766</v>
       </c>
       <c r="C47" s="7">
         <v>1</v>
@@ -4230,39 +4265,39 @@
         <v>118</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>31</v>
+        <v>164</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="K47" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="O47" s="7" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="P47" s="7"/>
       <c r="Q47" s="7"/>
       <c r="R47" s="7">
-        <v>31483</v>
+        <v>86982</v>
       </c>
       <c r="S47" s="7"/>
       <c r="T47" s="7"/>
@@ -4272,19 +4307,21 @@
       <c r="X47" s="7"/>
       <c r="Y47" s="7"/>
       <c r="Z47" s="8" t="s">
-        <v>134</v>
+        <v>198</v>
       </c>
       <c r="AA47" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AB47" s="7"/>
+      <c r="AB47" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:28">
       <c r="A48" s="3">
         <v>46</v>
       </c>
       <c r="B48" s="3">
-        <v>2025080447</v>
+        <v>2025080643</v>
       </c>
       <c r="C48" s="3">
         <v>1</v>
@@ -4296,39 +4333,41 @@
         <v>118</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>113</v>
+        <v>199</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>192</v>
+        <v>127</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
+        <v>200</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="L48" s="6" t="s">
-        <v>63</v>
+        <v>131</v>
       </c>
       <c r="M48" s="6" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
       <c r="R48" s="3">
-        <v>0</v>
-      </c>
-      <c r="S48" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>31483</v>
+      </c>
+      <c r="S48" s="3"/>
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
       <c r="V48" s="3"/>
@@ -4336,7 +4375,7 @@
       <c r="X48" s="3"/>
       <c r="Y48" s="3"/>
       <c r="Z48" s="6" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="AA48" s="3" t="s">
         <v>41</v>
@@ -4350,7 +4389,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="7">
-        <v>2025080035</v>
+        <v>2025080642</v>
       </c>
       <c r="C49" s="7">
         <v>1</v>
@@ -4362,41 +4401,43 @@
         <v>118</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>197</v>
+        <v>127</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>61</v>
+        <v>201</v>
       </c>
       <c r="K49" s="7" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>63</v>
+        <v>131</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="N49" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="O49" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="P49" s="7"/>
       <c r="Q49" s="7"/>
       <c r="R49" s="7">
-        <v>0</v>
-      </c>
-      <c r="S49" s="7"/>
+        <v>31483</v>
+      </c>
+      <c r="S49" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="T49" s="7"/>
       <c r="U49" s="7"/>
       <c r="V49" s="7"/>
@@ -4404,21 +4445,17 @@
       <c r="X49" s="7"/>
       <c r="Y49" s="7"/>
       <c r="Z49" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="AA49" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB49" s="7">
-        <v>1</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="AA49" s="7"/>
+      <c r="AB49" s="7"/>
     </row>
     <row r="50" spans="1:28">
       <c r="A50" s="3">
         <v>48</v>
       </c>
       <c r="B50" s="3">
-        <v>2025080425</v>
+        <v>2025080447</v>
       </c>
       <c r="C50" s="3">
         <v>1</v>
@@ -4433,13 +4470,13 @@
         <v>57</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>178</v>
+        <v>113</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>77</v>
+        <v>204</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -4447,10 +4484,10 @@
         <v>63</v>
       </c>
       <c r="M50" s="6" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="N50" s="6" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="O50" s="3" t="s">
         <v>40</v>
@@ -4484,7 +4521,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="7">
-        <v>2025080426</v>
+        <v>2025080035</v>
       </c>
       <c r="C51" s="7">
         <v>1</v>
@@ -4496,39 +4533,41 @@
         <v>118</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>178</v>
+        <v>208</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>77</v>
+        <v>209</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
+        <v>210</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K51" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="L51" s="8" t="s">
         <v>63</v>
       </c>
       <c r="M51" s="8" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="N51" s="8" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="O51" s="7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="P51" s="7"/>
       <c r="Q51" s="7"/>
       <c r="R51" s="7">
         <v>0</v>
       </c>
-      <c r="S51" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="S51" s="7"/>
       <c r="T51" s="7"/>
       <c r="U51" s="7"/>
       <c r="V51" s="7"/>
@@ -4536,19 +4575,21 @@
       <c r="X51" s="7"/>
       <c r="Y51" s="7"/>
       <c r="Z51" s="8" t="s">
-        <v>76</v>
+        <v>213</v>
       </c>
       <c r="AA51" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AB51" s="7"/>
+      <c r="AB51" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:28">
       <c r="A52" s="3">
         <v>50</v>
       </c>
       <c r="B52" s="3">
-        <v>2025080367</v>
+        <v>2025080425</v>
       </c>
       <c r="C52" s="3">
         <v>1</v>
@@ -4563,38 +4604,36 @@
         <v>57</v>
       </c>
       <c r="G52" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H52" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H52" s="3" t="s">
-        <v>181</v>
-      </c>
       <c r="I52" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
       <c r="L52" s="6" t="s">
         <v>63</v>
       </c>
       <c r="M52" s="6" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="O52" s="3" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3">
         <v>0</v>
       </c>
-      <c r="S52" s="3"/>
+      <c r="S52" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="T52" s="3"/>
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>
@@ -4602,19 +4641,21 @@
       <c r="X52" s="3"/>
       <c r="Y52" s="3"/>
       <c r="Z52" s="6" t="s">
-        <v>205</v>
+        <v>76</v>
       </c>
       <c r="AA52" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AB52" s="3"/>
+      <c r="AB52" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:28">
       <c r="A53" s="7">
         <v>51</v>
       </c>
       <c r="B53" s="7">
-        <v>2025080521</v>
+        <v>2025080426</v>
       </c>
       <c r="C53" s="7">
         <v>1</v>
@@ -4623,44 +4664,42 @@
         <v>29</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>206</v>
+        <v>118</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>208</v>
+        <v>77</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="J53" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="K53" s="7" t="s">
-        <v>62</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
       <c r="L53" s="8" t="s">
         <v>63</v>
       </c>
       <c r="M53" s="8" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="N53" s="8" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="O53" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="P53" s="7"/>
       <c r="Q53" s="7"/>
       <c r="R53" s="7">
         <v>0</v>
       </c>
-      <c r="S53" s="7"/>
+      <c r="S53" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="T53" s="7"/>
       <c r="U53" s="7"/>
       <c r="V53" s="7"/>
@@ -4668,21 +4707,19 @@
       <c r="X53" s="7"/>
       <c r="Y53" s="7"/>
       <c r="Z53" s="8" t="s">
-        <v>212</v>
+        <v>76</v>
       </c>
       <c r="AA53" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AB53" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB53" s="7"/>
     </row>
     <row r="54" spans="1:28">
       <c r="A54" s="3">
         <v>52</v>
       </c>
       <c r="B54" s="3">
-        <v>2025080636</v>
+        <v>2025080367</v>
       </c>
       <c r="C54" s="3">
         <v>1</v>
@@ -4691,42 +4728,44 @@
         <v>29</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>206</v>
+        <v>118</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>207</v>
+        <v>77</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
+        <v>214</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="L54" s="6" t="s">
         <v>63</v>
       </c>
       <c r="M54" s="6" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="N54" s="6" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
       <c r="R54" s="3">
         <v>0</v>
       </c>
-      <c r="S54" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="S54" s="3"/>
       <c r="T54" s="3"/>
       <c r="U54" s="3"/>
       <c r="V54" s="3"/>
@@ -4734,7 +4773,7 @@
       <c r="X54" s="3"/>
       <c r="Y54" s="3"/>
       <c r="Z54" s="6" t="s">
-        <v>76</v>
+        <v>217</v>
       </c>
       <c r="AA54" s="3" t="s">
         <v>41</v>
@@ -4746,7 +4785,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="7">
-        <v>2025080527</v>
+        <v>2025080636</v>
       </c>
       <c r="C55" s="7">
         <v>1</v>
@@ -4755,44 +4794,42 @@
         <v>29</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>31</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>207</v>
+        <v>166</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="J55" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="K55" s="7" t="s">
-        <v>62</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
       <c r="L55" s="8" t="s">
         <v>63</v>
       </c>
       <c r="M55" s="8" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="N55" s="8" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="O55" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="P55" s="7"/>
       <c r="Q55" s="7"/>
       <c r="R55" s="7">
         <v>0</v>
       </c>
-      <c r="S55" s="7"/>
+      <c r="S55" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="T55" s="7"/>
       <c r="U55" s="7"/>
       <c r="V55" s="7"/>
@@ -4800,45 +4837,179 @@
       <c r="X55" s="7"/>
       <c r="Y55" s="7"/>
       <c r="Z55" s="8" t="s">
-        <v>212</v>
+        <v>76</v>
       </c>
       <c r="AA55" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AB55" s="7"/>
+      <c r="AB55" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:28">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9"/>
-      <c r="K56" s="9"/>
-      <c r="L56" s="10"/>
-      <c r="M56" s="10"/>
-      <c r="N56" s="10"/>
-      <c r="O56" s="9"/>
-      <c r="P56" s="9"/>
-      <c r="Q56" s="9"/>
-      <c r="R56" s="9"/>
-      <c r="S56" s="9"/>
-      <c r="T56" s="9"/>
-      <c r="U56" s="9"/>
-      <c r="V56" s="9"/>
-      <c r="W56" s="9"/>
-      <c r="X56" s="9"/>
-      <c r="Y56" s="9"/>
-      <c r="Z56" s="10"/>
-      <c r="AA56" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="AB56" s="9">
-        <v>24</v>
+      <c r="A56" s="3">
+        <v>54</v>
+      </c>
+      <c r="B56" s="3">
+        <v>2025080521</v>
+      </c>
+      <c r="C56" s="3">
+        <v>1</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L56" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M56" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="N56" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="O56" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3">
+        <v>0</v>
+      </c>
+      <c r="S56" s="3"/>
+      <c r="T56" s="3"/>
+      <c r="U56" s="3"/>
+      <c r="V56" s="3"/>
+      <c r="W56" s="3"/>
+      <c r="X56" s="3"/>
+      <c r="Y56" s="3"/>
+      <c r="Z56" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA56" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB56" s="3"/>
+    </row>
+    <row r="57" spans="1:28">
+      <c r="A57" s="7">
+        <v>55</v>
+      </c>
+      <c r="B57" s="7">
+        <v>2025080527</v>
+      </c>
+      <c r="C57" s="7">
+        <v>1</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="J57" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K57" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L57" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="M57" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="N57" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="O57" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P57" s="7"/>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="7">
+        <v>0</v>
+      </c>
+      <c r="S57" s="7"/>
+      <c r="T57" s="7"/>
+      <c r="U57" s="7"/>
+      <c r="V57" s="7"/>
+      <c r="W57" s="7"/>
+      <c r="X57" s="7"/>
+      <c r="Y57" s="7"/>
+      <c r="Z57" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA57" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB57" s="7"/>
+    </row>
+    <row r="58" spans="1:28">
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="10"/>
+      <c r="M58" s="10"/>
+      <c r="N58" s="10"/>
+      <c r="O58" s="9"/>
+      <c r="P58" s="9"/>
+      <c r="Q58" s="9"/>
+      <c r="R58" s="9"/>
+      <c r="S58" s="9"/>
+      <c r="T58" s="9"/>
+      <c r="U58" s="9"/>
+      <c r="V58" s="9"/>
+      <c r="W58" s="9"/>
+      <c r="X58" s="9"/>
+      <c r="Y58" s="9"/>
+      <c r="Z58" s="10"/>
+      <c r="AA58" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="AB58" s="9">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit - 08181803
</commit_message>
<xml_diff>
--- a/IM/202508_Service_Count_Report.xlsx
+++ b/IM/202508_Service_Count_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AA$237</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AA$238</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="703">
   <si>
     <t>服務次數統計表        篩選月份：202508</t>
   </si>
@@ -532,29 +532,29 @@
     <t>12:30:00</t>
   </si>
   <si>
+    <t>13:28:00</t>
+  </si>
+  <si>
+    <t>THILF02259</t>
+  </si>
+  <si>
+    <t>新北市三重區中華路18號</t>
+  </si>
+  <si>
+    <t>三重興華店</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119011857
+換上8119012492</t>
+  </si>
+  <si>
     <t>13:29:00</t>
-  </si>
-  <si>
-    <t>THILF02259</t>
-  </si>
-  <si>
-    <t>新北市三重區中華路18號</t>
-  </si>
-  <si>
-    <t>三重興華店</t>
   </si>
   <si>
     <t>更換掃描槍
 換下8119011905
 換上8119012491</t>
-  </si>
-  <si>
-    <t>13:28:00</t>
-  </si>
-  <si>
-    <t>更換掃描槍
-換下8119011857
-換上8119012492</t>
   </si>
   <si>
     <t>2025-08-11</t>
@@ -1968,6 +1968,21 @@
     <t>狄澤洋</t>
   </si>
   <si>
+    <t>17:01:00</t>
+  </si>
+  <si>
+    <t>T301800045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">台芝國際股份有限公司 </t>
+  </si>
+  <si>
+    <t>新北市三重區光復路一段82之8號8樓</t>
+  </si>
+  <si>
+    <t>A4紙8 15已送達</t>
+  </si>
+  <si>
     <t>17:33:00</t>
   </si>
   <si>
@@ -2006,7 +2021,7 @@
     <t>2025-08-17</t>
   </si>
   <si>
-    <t>15:45:00</t>
+    <t>14:33:00</t>
   </si>
   <si>
     <t>THILF03955</t>
@@ -2016,14 +2031,14 @@
   </si>
   <si>
     <t>板橋海龍店</t>
-  </si>
-  <si>
-    <t>14:33:00</t>
   </si>
   <si>
     <t>更換SC第一顆硬碟無備份還原
 H20250805
 已通知檢查代收</t>
+  </si>
+  <si>
+    <t>15:45:00</t>
   </si>
   <si>
     <t>12:15:00</t>
@@ -2590,10 +2605,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB237"/>
+  <dimension ref="A1:AB238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A237" sqref="A237"/>
+      <selection activeCell="A238" sqref="A238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4739,7 +4754,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="3">
-        <v>2025080366</v>
+        <v>2025080365</v>
       </c>
       <c r="C32" s="3">
         <v>1</v>
@@ -4807,7 +4822,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="7">
-        <v>2025080365</v>
+        <v>2025080366</v>
       </c>
       <c r="C33" s="7">
         <v>1</v>
@@ -8619,7 +8634,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="3">
-        <v>2025081551</v>
+        <v>2025081550</v>
       </c>
       <c r="C90" s="3">
         <v>1</v>
@@ -8656,7 +8671,7 @@
       </c>
       <c r="N90" s="6"/>
       <c r="O90" s="3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="P90" s="3"/>
       <c r="Q90" s="3">
@@ -8665,7 +8680,9 @@
       <c r="R90" s="3">
         <v>41000</v>
       </c>
-      <c r="S90" s="3"/>
+      <c r="S90" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T90" s="3"/>
       <c r="U90" s="3"/>
       <c r="V90" s="3"/>
@@ -8687,7 +8704,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="7">
-        <v>2025081550</v>
+        <v>2025081551</v>
       </c>
       <c r="C91" s="7">
         <v>1</v>
@@ -8724,7 +8741,7 @@
       </c>
       <c r="N91" s="8"/>
       <c r="O91" s="7" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="P91" s="7"/>
       <c r="Q91" s="7">
@@ -8733,9 +8750,7 @@
       <c r="R91" s="7">
         <v>41000</v>
       </c>
-      <c r="S91" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S91" s="7"/>
       <c r="T91" s="7"/>
       <c r="U91" s="7"/>
       <c r="V91" s="7"/>
@@ -9881,7 +9896,7 @@
         <v>106</v>
       </c>
       <c r="B108" s="3">
-        <v>2025080704</v>
+        <v>2025080705</v>
       </c>
       <c r="C108" s="3">
         <v>1</v>
@@ -9920,16 +9935,14 @@
         <v>429</v>
       </c>
       <c r="O108" s="3" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="P108" s="3"/>
       <c r="Q108" s="3"/>
       <c r="R108" s="3">
         <v>7108</v>
       </c>
-      <c r="S108" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S108" s="3"/>
       <c r="T108" s="3"/>
       <c r="U108" s="3"/>
       <c r="V108" s="3"/>
@@ -9939,15 +9952,19 @@
       <c r="Z108" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="AA108" s="3"/>
-      <c r="AB108" s="3"/>
+      <c r="AA108" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB108" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="109" spans="1:28">
       <c r="A109" s="7">
         <v>107</v>
       </c>
       <c r="B109" s="7">
-        <v>2025080705</v>
+        <v>2025080704</v>
       </c>
       <c r="C109" s="7">
         <v>1</v>
@@ -9986,14 +10003,16 @@
         <v>429</v>
       </c>
       <c r="O109" s="7" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="P109" s="7"/>
       <c r="Q109" s="7"/>
       <c r="R109" s="7">
         <v>7108</v>
       </c>
-      <c r="S109" s="7"/>
+      <c r="S109" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T109" s="7"/>
       <c r="U109" s="7"/>
       <c r="V109" s="7"/>
@@ -10003,9 +10022,7 @@
       <c r="Z109" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="AA109" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA109" s="7"/>
       <c r="AB109" s="7"/>
     </row>
     <row r="110" spans="1:28">
@@ -11033,7 +11050,7 @@
         <v>123</v>
       </c>
       <c r="B125" s="7">
-        <v>2025080863</v>
+        <v>2025080864</v>
       </c>
       <c r="C125" s="7">
         <v>1</v>
@@ -11072,16 +11089,14 @@
         <v>459</v>
       </c>
       <c r="O125" s="7" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="P125" s="7"/>
       <c r="Q125" s="7"/>
       <c r="R125" s="7">
         <v>131744</v>
       </c>
-      <c r="S125" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S125" s="7"/>
       <c r="T125" s="7"/>
       <c r="U125" s="7"/>
       <c r="V125" s="7"/>
@@ -11103,7 +11118,7 @@
         <v>124</v>
       </c>
       <c r="B126" s="3">
-        <v>2025080864</v>
+        <v>2025080863</v>
       </c>
       <c r="C126" s="3">
         <v>1</v>
@@ -11142,14 +11157,16 @@
         <v>459</v>
       </c>
       <c r="O126" s="3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="P126" s="3"/>
       <c r="Q126" s="3"/>
       <c r="R126" s="3">
         <v>131744</v>
       </c>
-      <c r="S126" s="3"/>
+      <c r="S126" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T126" s="3"/>
       <c r="U126" s="3"/>
       <c r="V126" s="3"/>
@@ -14085,7 +14102,7 @@
         <v>168</v>
       </c>
       <c r="B170" s="3">
-        <v>2025081973</v>
+        <v>2025081974</v>
       </c>
       <c r="C170" s="3">
         <v>1</v>
@@ -14122,16 +14139,14 @@
       </c>
       <c r="N170" s="6"/>
       <c r="O170" s="3" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="P170" s="3"/>
       <c r="Q170" s="3"/>
       <c r="R170" s="3">
         <v>80962</v>
       </c>
-      <c r="S170" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S170" s="3"/>
       <c r="T170" s="3"/>
       <c r="U170" s="3"/>
       <c r="V170" s="3"/>
@@ -14153,7 +14168,7 @@
         <v>169</v>
       </c>
       <c r="B171" s="7">
-        <v>2025081974</v>
+        <v>2025081973</v>
       </c>
       <c r="C171" s="7">
         <v>1</v>
@@ -14190,14 +14205,16 @@
       </c>
       <c r="N171" s="8"/>
       <c r="O171" s="7" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="P171" s="7"/>
       <c r="Q171" s="7"/>
       <c r="R171" s="7">
         <v>80962</v>
       </c>
-      <c r="S171" s="7"/>
+      <c r="S171" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T171" s="7"/>
       <c r="U171" s="7"/>
       <c r="V171" s="7"/>
@@ -14899,7 +14916,7 @@
         <v>180</v>
       </c>
       <c r="B182" s="3">
-        <v>2025081292</v>
+        <v>2025081293</v>
       </c>
       <c r="C182" s="3">
         <v>1</v>
@@ -14938,16 +14955,14 @@
         <v>509</v>
       </c>
       <c r="O182" s="3" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="P182" s="3"/>
       <c r="Q182" s="3"/>
       <c r="R182" s="3">
         <v>3085</v>
       </c>
-      <c r="S182" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S182" s="3"/>
       <c r="T182" s="3"/>
       <c r="U182" s="3"/>
       <c r="V182" s="3"/>
@@ -14957,15 +14972,19 @@
       <c r="Z182" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="AA182" s="3"/>
-      <c r="AB182" s="3"/>
+      <c r="AA182" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB182" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="183" spans="1:28">
       <c r="A183" s="7">
         <v>181</v>
       </c>
       <c r="B183" s="7">
-        <v>2025081293</v>
+        <v>2025081292</v>
       </c>
       <c r="C183" s="7">
         <v>1</v>
@@ -15004,14 +15023,16 @@
         <v>509</v>
       </c>
       <c r="O183" s="7" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="P183" s="7"/>
       <c r="Q183" s="7"/>
       <c r="R183" s="7">
         <v>3085</v>
       </c>
-      <c r="S183" s="7"/>
+      <c r="S183" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T183" s="7"/>
       <c r="U183" s="7"/>
       <c r="V183" s="7"/>
@@ -15021,9 +15042,7 @@
       <c r="Z183" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="AA183" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA183" s="7"/>
       <c r="AB183" s="7"/>
     </row>
     <row r="184" spans="1:28">
@@ -17099,7 +17118,7 @@
         <v>213</v>
       </c>
       <c r="B215" s="7">
-        <v>2025081824</v>
+        <v>2025082186</v>
       </c>
       <c r="C215" s="7">
         <v>1</v>
@@ -17111,50 +17130,52 @@
         <v>632</v>
       </c>
       <c r="F215" s="7" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="G215" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="H215" s="7" t="s">
         <v>633</v>
       </c>
-      <c r="H215" s="7" t="s">
+      <c r="I215" s="7" t="s">
         <v>634</v>
       </c>
-      <c r="I215" s="7" t="s">
-        <v>635</v>
-      </c>
       <c r="J215" s="7" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="K215" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L215" s="8" t="s">
+        <v>635</v>
+      </c>
+      <c r="M215" s="8" t="s">
         <v>636</v>
       </c>
-      <c r="M215" s="8" t="s">
-        <v>637</v>
-      </c>
       <c r="N215" s="8" t="s">
-        <v>450</v>
+        <v>632</v>
       </c>
       <c r="O215" s="7" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="P215" s="7"/>
-      <c r="Q215" s="7">
-        <v>4667</v>
-      </c>
+      <c r="Q215" s="7"/>
       <c r="R215" s="7">
-        <v>56483</v>
+        <v>140764</v>
       </c>
       <c r="S215" s="7"/>
       <c r="T215" s="7"/>
       <c r="U215" s="7"/>
-      <c r="V215" s="7"/>
+      <c r="V215" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="W215" s="7"/>
       <c r="X215" s="7"/>
       <c r="Y215" s="7"/>
-      <c r="Z215" s="8"/>
+      <c r="Z215" s="8" t="s">
+        <v>637</v>
+      </c>
       <c r="AA215" s="7" t="s">
         <v>40</v>
       </c>
@@ -17167,7 +17188,7 @@
         <v>214</v>
       </c>
       <c r="B216" s="3">
-        <v>2025081823</v>
+        <v>2025081824</v>
       </c>
       <c r="C216" s="3">
         <v>1</v>
@@ -17182,13 +17203,13 @@
         <v>47</v>
       </c>
       <c r="G216" s="3" t="s">
-        <v>633</v>
+        <v>638</v>
       </c>
       <c r="H216" s="3" t="s">
-        <v>634</v>
+        <v>639</v>
       </c>
       <c r="I216" s="3" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="J216" s="3" t="s">
         <v>133</v>
@@ -17197,10 +17218,10 @@
         <v>36</v>
       </c>
       <c r="L216" s="6" t="s">
-        <v>636</v>
+        <v>641</v>
       </c>
       <c r="M216" s="6" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
       <c r="N216" s="6" t="s">
         <v>450</v>
@@ -17210,10 +17231,10 @@
       </c>
       <c r="P216" s="3"/>
       <c r="Q216" s="3">
-        <v>7042</v>
+        <v>4667</v>
       </c>
       <c r="R216" s="3">
-        <v>96734</v>
+        <v>56483</v>
       </c>
       <c r="S216" s="3"/>
       <c r="T216" s="3"/>
@@ -17235,7 +17256,7 @@
         <v>215</v>
       </c>
       <c r="B217" s="7">
-        <v>2025081304</v>
+        <v>2025081823</v>
       </c>
       <c r="C217" s="7">
         <v>1</v>
@@ -17247,39 +17268,41 @@
         <v>632</v>
       </c>
       <c r="F217" s="7" t="s">
-        <v>189</v>
+        <v>47</v>
       </c>
       <c r="G217" s="7" t="s">
-        <v>415</v>
+        <v>638</v>
       </c>
       <c r="H217" s="7" t="s">
         <v>639</v>
       </c>
       <c r="I217" s="7" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="J217" s="7" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="K217" s="7" t="s">
-        <v>144</v>
+        <v>36</v>
       </c>
       <c r="L217" s="8" t="s">
-        <v>145</v>
+        <v>641</v>
       </c>
       <c r="M217" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="N217" s="8" t="s">
-        <v>642</v>
+        <v>450</v>
       </c>
       <c r="O217" s="7" t="s">
-        <v>125</v>
+        <v>39</v>
       </c>
       <c r="P217" s="7"/>
-      <c r="Q217" s="7"/>
+      <c r="Q217" s="7">
+        <v>7042</v>
+      </c>
       <c r="R217" s="7">
-        <v>0</v>
+        <v>96734</v>
       </c>
       <c r="S217" s="7"/>
       <c r="T217" s="7"/>
@@ -17288,9 +17311,7 @@
       <c r="W217" s="7"/>
       <c r="X217" s="7"/>
       <c r="Y217" s="7"/>
-      <c r="Z217" s="8" t="s">
-        <v>643</v>
-      </c>
+      <c r="Z217" s="8"/>
       <c r="AA217" s="7" t="s">
         <v>40</v>
       </c>
@@ -17321,10 +17342,10 @@
         <v>415</v>
       </c>
       <c r="H218" s="3" t="s">
-        <v>639</v>
+        <v>644</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="J218" s="3"/>
       <c r="K218" s="3"/>
@@ -17332,10 +17353,10 @@
         <v>145</v>
       </c>
       <c r="M218" s="6" t="s">
-        <v>641</v>
+        <v>646</v>
       </c>
       <c r="N218" s="6" t="s">
-        <v>642</v>
+        <v>647</v>
       </c>
       <c r="O218" s="3" t="s">
         <v>54</v>
@@ -17360,14 +17381,16 @@
       <c r="AA218" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AB218" s="3"/>
+      <c r="AB218" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="219" spans="1:28">
       <c r="A219" s="7">
         <v>217</v>
       </c>
       <c r="B219" s="7">
-        <v>2025082021</v>
+        <v>2025081304</v>
       </c>
       <c r="C219" s="7">
         <v>1</v>
@@ -17379,39 +17402,41 @@
         <v>632</v>
       </c>
       <c r="F219" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G219" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="H219" s="7" t="s">
         <v>644</v>
       </c>
-      <c r="G219" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="H219" s="7" t="s">
+      <c r="I219" s="7" t="s">
         <v>645</v>
       </c>
-      <c r="I219" s="7" t="s">
-        <v>646</v>
-      </c>
-      <c r="J219" s="7"/>
-      <c r="K219" s="7"/>
+      <c r="J219" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="K219" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="L219" s="8" t="s">
         <v>145</v>
       </c>
       <c r="M219" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="N219" s="8" t="s">
         <v>647</v>
       </c>
-      <c r="N219" s="8" t="s">
-        <v>648</v>
-      </c>
       <c r="O219" s="7" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="P219" s="7"/>
       <c r="Q219" s="7"/>
       <c r="R219" s="7">
         <v>0</v>
       </c>
-      <c r="S219" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S219" s="7"/>
       <c r="T219" s="7"/>
       <c r="U219" s="7"/>
       <c r="V219" s="7"/>
@@ -17419,14 +17444,12 @@
       <c r="X219" s="7"/>
       <c r="Y219" s="7"/>
       <c r="Z219" s="8" t="s">
-        <v>161</v>
+        <v>648</v>
       </c>
       <c r="AA219" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AB219" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB219" s="7"/>
     </row>
     <row r="220" spans="1:28">
       <c r="A220" s="3">
@@ -17445,16 +17468,16 @@
         <v>632</v>
       </c>
       <c r="F220" s="3" t="s">
-        <v>644</v>
+        <v>649</v>
       </c>
       <c r="G220" s="3" t="s">
         <v>326</v>
       </c>
       <c r="H220" s="3" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>646</v>
+        <v>651</v>
       </c>
       <c r="J220" s="3" t="s">
         <v>175</v>
@@ -17466,10 +17489,10 @@
         <v>145</v>
       </c>
       <c r="M220" s="6" t="s">
-        <v>647</v>
+        <v>652</v>
       </c>
       <c r="N220" s="6" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
       <c r="O220" s="3" t="s">
         <v>125</v>
@@ -17487,19 +17510,21 @@
       <c r="X220" s="3"/>
       <c r="Y220" s="3"/>
       <c r="Z220" s="6" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
       <c r="AA220" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AB220" s="3"/>
+      <c r="AB220" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="221" spans="1:28">
       <c r="A221" s="7">
         <v>219</v>
       </c>
       <c r="B221" s="7">
-        <v>2025081585</v>
+        <v>2025082021</v>
       </c>
       <c r="C221" s="7">
         <v>1</v>
@@ -17511,16 +17536,16 @@
         <v>632</v>
       </c>
       <c r="F221" s="7" t="s">
-        <v>239</v>
+        <v>649</v>
       </c>
       <c r="G221" s="7" t="s">
-        <v>415</v>
+        <v>326</v>
       </c>
       <c r="H221" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="I221" s="7" t="s">
         <v>651</v>
-      </c>
-      <c r="I221" s="7" t="s">
-        <v>652</v>
       </c>
       <c r="J221" s="7"/>
       <c r="K221" s="7"/>
@@ -17528,10 +17553,10 @@
         <v>145</v>
       </c>
       <c r="M221" s="8" t="s">
+        <v>652</v>
+      </c>
+      <c r="N221" s="8" t="s">
         <v>653</v>
-      </c>
-      <c r="N221" s="8" t="s">
-        <v>654</v>
       </c>
       <c r="O221" s="7" t="s">
         <v>54</v>
@@ -17556,16 +17581,14 @@
       <c r="AA221" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AB221" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB221" s="7"/>
     </row>
     <row r="222" spans="1:28">
       <c r="A222" s="3">
         <v>220</v>
       </c>
       <c r="B222" s="3">
-        <v>2025081584</v>
+        <v>2025081585</v>
       </c>
       <c r="C222" s="3">
         <v>1</v>
@@ -17580,7 +17603,7 @@
         <v>239</v>
       </c>
       <c r="G222" s="3" t="s">
-        <v>655</v>
+        <v>415</v>
       </c>
       <c r="H222" s="3" t="s">
         <v>656</v>
@@ -17617,7 +17640,7 @@
       <c r="X222" s="3"/>
       <c r="Y222" s="3"/>
       <c r="Z222" s="6" t="s">
-        <v>660</v>
+        <v>161</v>
       </c>
       <c r="AA222" s="3" t="s">
         <v>40</v>
@@ -17631,7 +17654,7 @@
         <v>221</v>
       </c>
       <c r="B223" s="7">
-        <v>2025081467</v>
+        <v>2025081584</v>
       </c>
       <c r="C223" s="7">
         <v>1</v>
@@ -17643,13 +17666,13 @@
         <v>632</v>
       </c>
       <c r="F223" s="7" t="s">
-        <v>189</v>
+        <v>239</v>
       </c>
       <c r="G223" s="7" t="s">
+        <v>660</v>
+      </c>
+      <c r="H223" s="7" t="s">
         <v>661</v>
-      </c>
-      <c r="H223" s="7" t="s">
-        <v>149</v>
       </c>
       <c r="I223" s="7" t="s">
         <v>662</v>
@@ -17683,7 +17706,7 @@
       <c r="X223" s="7"/>
       <c r="Y223" s="7"/>
       <c r="Z223" s="8" t="s">
-        <v>161</v>
+        <v>665</v>
       </c>
       <c r="AA223" s="7" t="s">
         <v>40</v>
@@ -17697,7 +17720,7 @@
         <v>222</v>
       </c>
       <c r="B224" s="3">
-        <v>2025080889</v>
+        <v>2025081467</v>
       </c>
       <c r="C224" s="3">
         <v>1</v>
@@ -17709,23 +17732,19 @@
         <v>632</v>
       </c>
       <c r="F224" s="3" t="s">
-        <v>232</v>
+        <v>189</v>
       </c>
       <c r="G224" s="3" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="H224" s="3" t="s">
-        <v>666</v>
+        <v>149</v>
       </c>
       <c r="I224" s="3" t="s">
         <v>667</v>
       </c>
-      <c r="J224" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="K224" s="3" t="s">
-        <v>144</v>
-      </c>
+      <c r="J224" s="3"/>
+      <c r="K224" s="3"/>
       <c r="L224" s="6" t="s">
         <v>145</v>
       </c>
@@ -17736,14 +17755,16 @@
         <v>669</v>
       </c>
       <c r="O224" s="3" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="P224" s="3"/>
       <c r="Q224" s="3"/>
       <c r="R224" s="3">
         <v>0</v>
       </c>
-      <c r="S224" s="3"/>
+      <c r="S224" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T224" s="3"/>
       <c r="U224" s="3"/>
       <c r="V224" s="3"/>
@@ -17751,7 +17772,7 @@
       <c r="X224" s="3"/>
       <c r="Y224" s="3"/>
       <c r="Z224" s="6" t="s">
-        <v>670</v>
+        <v>161</v>
       </c>
       <c r="AA224" s="3" t="s">
         <v>40</v>
@@ -17765,7 +17786,7 @@
         <v>223</v>
       </c>
       <c r="B225" s="7">
-        <v>2025081062</v>
+        <v>2025080889</v>
       </c>
       <c r="C225" s="7">
         <v>1</v>
@@ -17780,36 +17801,38 @@
         <v>232</v>
       </c>
       <c r="G225" s="7" t="s">
+        <v>670</v>
+      </c>
+      <c r="H225" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="H225" s="7" t="s">
-        <v>645</v>
-      </c>
       <c r="I225" s="7" t="s">
-        <v>667</v>
-      </c>
-      <c r="J225" s="7"/>
-      <c r="K225" s="7"/>
+        <v>672</v>
+      </c>
+      <c r="J225" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="K225" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="L225" s="8" t="s">
         <v>145</v>
       </c>
       <c r="M225" s="8" t="s">
-        <v>668</v>
+        <v>673</v>
       </c>
       <c r="N225" s="8" t="s">
-        <v>669</v>
+        <v>674</v>
       </c>
       <c r="O225" s="7" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="P225" s="7"/>
       <c r="Q225" s="7"/>
       <c r="R225" s="7">
         <v>0</v>
       </c>
-      <c r="S225" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S225" s="7"/>
       <c r="T225" s="7"/>
       <c r="U225" s="7"/>
       <c r="V225" s="7"/>
@@ -17817,19 +17840,21 @@
       <c r="X225" s="7"/>
       <c r="Y225" s="7"/>
       <c r="Z225" s="8" t="s">
-        <v>161</v>
+        <v>675</v>
       </c>
       <c r="AA225" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AB225" s="7"/>
+      <c r="AB225" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="226" spans="1:28">
       <c r="A226" s="3">
         <v>224</v>
       </c>
       <c r="B226" s="3">
-        <v>2025082114</v>
+        <v>2025081062</v>
       </c>
       <c r="C226" s="3">
         <v>1</v>
@@ -17841,23 +17866,19 @@
         <v>632</v>
       </c>
       <c r="F226" s="3" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="G226" s="3" t="s">
-        <v>326</v>
+        <v>676</v>
       </c>
       <c r="H226" s="3" t="s">
-        <v>215</v>
+        <v>655</v>
       </c>
       <c r="I226" s="3" t="s">
         <v>672</v>
       </c>
-      <c r="J226" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="K226" s="3" t="s">
-        <v>144</v>
-      </c>
+      <c r="J226" s="3"/>
+      <c r="K226" s="3"/>
       <c r="L226" s="6" t="s">
         <v>145</v>
       </c>
@@ -17868,14 +17889,16 @@
         <v>674</v>
       </c>
       <c r="O226" s="3" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="P226" s="3"/>
       <c r="Q226" s="3"/>
       <c r="R226" s="3">
         <v>0</v>
       </c>
-      <c r="S226" s="3"/>
+      <c r="S226" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T226" s="3"/>
       <c r="U226" s="3"/>
       <c r="V226" s="3"/>
@@ -17883,21 +17906,19 @@
       <c r="X226" s="3"/>
       <c r="Y226" s="3"/>
       <c r="Z226" s="6" t="s">
-        <v>675</v>
+        <v>161</v>
       </c>
       <c r="AA226" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AB226" s="3">
-        <v>1</v>
-      </c>
+      <c r="AB226" s="3"/>
     </row>
     <row r="227" spans="1:28">
       <c r="A227" s="7">
         <v>225</v>
       </c>
       <c r="B227" s="7">
-        <v>2025082122</v>
+        <v>2025082114</v>
       </c>
       <c r="C227" s="7">
         <v>1</v>
@@ -17918,30 +17939,32 @@
         <v>215</v>
       </c>
       <c r="I227" s="7" t="s">
-        <v>672</v>
-      </c>
-      <c r="J227" s="7"/>
-      <c r="K227" s="7"/>
+        <v>677</v>
+      </c>
+      <c r="J227" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="K227" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="L227" s="8" t="s">
         <v>145</v>
       </c>
       <c r="M227" s="8" t="s">
-        <v>673</v>
+        <v>678</v>
       </c>
       <c r="N227" s="8" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="O227" s="7" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="P227" s="7"/>
       <c r="Q227" s="7"/>
       <c r="R227" s="7">
         <v>0</v>
       </c>
-      <c r="S227" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S227" s="7"/>
       <c r="T227" s="7"/>
       <c r="U227" s="7"/>
       <c r="V227" s="7"/>
@@ -17949,19 +17972,21 @@
       <c r="X227" s="7"/>
       <c r="Y227" s="7"/>
       <c r="Z227" s="8" t="s">
-        <v>161</v>
+        <v>680</v>
       </c>
       <c r="AA227" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AB227" s="7"/>
+      <c r="AB227" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="228" spans="1:28">
       <c r="A228" s="3">
         <v>226</v>
       </c>
       <c r="B228" s="3">
-        <v>2025081870</v>
+        <v>2025082122</v>
       </c>
       <c r="C228" s="3">
         <v>1</v>
@@ -17982,32 +18007,30 @@
         <v>215</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>672</v>
-      </c>
-      <c r="J228" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="K228" s="3" t="s">
-        <v>144</v>
-      </c>
+        <v>677</v>
+      </c>
+      <c r="J228" s="3"/>
+      <c r="K228" s="3"/>
       <c r="L228" s="6" t="s">
         <v>145</v>
       </c>
       <c r="M228" s="6" t="s">
-        <v>673</v>
+        <v>678</v>
       </c>
       <c r="N228" s="6" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="O228" s="3" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="P228" s="3"/>
       <c r="Q228" s="3"/>
       <c r="R228" s="3">
         <v>0</v>
       </c>
-      <c r="S228" s="3"/>
+      <c r="S228" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T228" s="3"/>
       <c r="U228" s="3"/>
       <c r="V228" s="3"/>
@@ -18015,7 +18038,7 @@
       <c r="X228" s="3"/>
       <c r="Y228" s="3"/>
       <c r="Z228" s="6" t="s">
-        <v>676</v>
+        <v>161</v>
       </c>
       <c r="AA228" s="3" t="s">
         <v>40</v>
@@ -18027,7 +18050,7 @@
         <v>227</v>
       </c>
       <c r="B229" s="7">
-        <v>2025080521</v>
+        <v>2025081870</v>
       </c>
       <c r="C229" s="7">
         <v>1</v>
@@ -18039,16 +18062,16 @@
         <v>632</v>
       </c>
       <c r="F229" s="7" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="G229" s="7" t="s">
-        <v>245</v>
+        <v>326</v>
       </c>
       <c r="H229" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="I229" s="7" t="s">
         <v>677</v>
-      </c>
-      <c r="I229" s="7" t="s">
-        <v>678</v>
       </c>
       <c r="J229" s="7" t="s">
         <v>143</v>
@@ -18060,10 +18083,10 @@
         <v>145</v>
       </c>
       <c r="M229" s="8" t="s">
+        <v>678</v>
+      </c>
+      <c r="N229" s="8" t="s">
         <v>679</v>
-      </c>
-      <c r="N229" s="8" t="s">
-        <v>680</v>
       </c>
       <c r="O229" s="7" t="s">
         <v>125</v>
@@ -18086,16 +18109,14 @@
       <c r="AA229" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AB229" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB229" s="7"/>
     </row>
     <row r="230" spans="1:28">
       <c r="A230" s="3">
         <v>228</v>
       </c>
       <c r="B230" s="3">
-        <v>2025080527</v>
+        <v>2025080521</v>
       </c>
       <c r="C230" s="3">
         <v>1</v>
@@ -18113,10 +18134,10 @@
         <v>245</v>
       </c>
       <c r="H230" s="3" t="s">
-        <v>282</v>
+        <v>682</v>
       </c>
       <c r="I230" s="3" t="s">
-        <v>678</v>
+        <v>683</v>
       </c>
       <c r="J230" s="3" t="s">
         <v>143</v>
@@ -18128,10 +18149,10 @@
         <v>145</v>
       </c>
       <c r="M230" s="6" t="s">
-        <v>679</v>
+        <v>684</v>
       </c>
       <c r="N230" s="6" t="s">
-        <v>680</v>
+        <v>685</v>
       </c>
       <c r="O230" s="3" t="s">
         <v>125</v>
@@ -18149,19 +18170,21 @@
       <c r="X230" s="3"/>
       <c r="Y230" s="3"/>
       <c r="Z230" s="6" t="s">
-        <v>681</v>
+        <v>686</v>
       </c>
       <c r="AA230" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AB230" s="3"/>
+      <c r="AB230" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="231" spans="1:28">
       <c r="A231" s="7">
         <v>229</v>
       </c>
       <c r="B231" s="7">
-        <v>2025080636</v>
+        <v>2025080527</v>
       </c>
       <c r="C231" s="7">
         <v>1</v>
@@ -18179,33 +18202,35 @@
         <v>245</v>
       </c>
       <c r="H231" s="7" t="s">
-        <v>246</v>
+        <v>282</v>
       </c>
       <c r="I231" s="7" t="s">
-        <v>678</v>
-      </c>
-      <c r="J231" s="7"/>
-      <c r="K231" s="7"/>
+        <v>683</v>
+      </c>
+      <c r="J231" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="K231" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="L231" s="8" t="s">
         <v>145</v>
       </c>
       <c r="M231" s="8" t="s">
-        <v>679</v>
+        <v>684</v>
       </c>
       <c r="N231" s="8" t="s">
-        <v>680</v>
+        <v>685</v>
       </c>
       <c r="O231" s="7" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="P231" s="7"/>
       <c r="Q231" s="7"/>
       <c r="R231" s="7">
         <v>0</v>
       </c>
-      <c r="S231" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S231" s="7"/>
       <c r="T231" s="7"/>
       <c r="U231" s="7"/>
       <c r="V231" s="7"/>
@@ -18213,7 +18238,7 @@
       <c r="X231" s="7"/>
       <c r="Y231" s="7"/>
       <c r="Z231" s="8" t="s">
-        <v>161</v>
+        <v>686</v>
       </c>
       <c r="AA231" s="7" t="s">
         <v>40</v>
@@ -18225,7 +18250,7 @@
         <v>230</v>
       </c>
       <c r="B232" s="3">
-        <v>2025080946</v>
+        <v>2025080636</v>
       </c>
       <c r="C232" s="3">
         <v>1</v>
@@ -18237,41 +18262,39 @@
         <v>632</v>
       </c>
       <c r="F232" s="3" t="s">
-        <v>232</v>
+        <v>94</v>
       </c>
       <c r="G232" s="3" t="s">
-        <v>682</v>
+        <v>245</v>
       </c>
       <c r="H232" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="I232" s="3" t="s">
         <v>683</v>
       </c>
-      <c r="I232" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="J232" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="K232" s="3" t="s">
-        <v>144</v>
-      </c>
+      <c r="J232" s="3"/>
+      <c r="K232" s="3"/>
       <c r="L232" s="6" t="s">
         <v>145</v>
       </c>
       <c r="M232" s="6" t="s">
+        <v>684</v>
+      </c>
+      <c r="N232" s="6" t="s">
         <v>685</v>
       </c>
-      <c r="N232" s="6" t="s">
-        <v>686</v>
-      </c>
       <c r="O232" s="3" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="P232" s="3"/>
       <c r="Q232" s="3"/>
       <c r="R232" s="3">
         <v>0</v>
       </c>
-      <c r="S232" s="3"/>
+      <c r="S232" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T232" s="3"/>
       <c r="U232" s="3"/>
       <c r="V232" s="3"/>
@@ -18279,21 +18302,19 @@
       <c r="X232" s="3"/>
       <c r="Y232" s="3"/>
       <c r="Z232" s="6" t="s">
-        <v>687</v>
+        <v>161</v>
       </c>
       <c r="AA232" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AB232" s="3">
-        <v>1</v>
-      </c>
+      <c r="AB232" s="3"/>
     </row>
     <row r="233" spans="1:28">
       <c r="A233" s="7">
         <v>231</v>
       </c>
       <c r="B233" s="7">
-        <v>2025081053</v>
+        <v>2025080946</v>
       </c>
       <c r="C233" s="7">
         <v>1</v>
@@ -18308,27 +18329,31 @@
         <v>232</v>
       </c>
       <c r="G233" s="7" t="s">
-        <v>682</v>
+        <v>687</v>
       </c>
       <c r="H233" s="7" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
       <c r="I233" s="7" t="s">
-        <v>684</v>
-      </c>
-      <c r="J233" s="7"/>
-      <c r="K233" s="7"/>
+        <v>689</v>
+      </c>
+      <c r="J233" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="K233" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="L233" s="8" t="s">
         <v>145</v>
       </c>
       <c r="M233" s="8" t="s">
-        <v>685</v>
+        <v>690</v>
       </c>
       <c r="N233" s="8" t="s">
-        <v>686</v>
+        <v>691</v>
       </c>
       <c r="O233" s="7" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="P233" s="7"/>
       <c r="Q233" s="7"/>
@@ -18341,23 +18366,23 @@
       <c r="V233" s="7"/>
       <c r="W233" s="7"/>
       <c r="X233" s="7"/>
-      <c r="Y233" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="Y233" s="7"/>
       <c r="Z233" s="8" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="AA233" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AB233" s="7"/>
+      <c r="AB233" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="234" spans="1:28">
       <c r="A234" s="3">
         <v>232</v>
       </c>
       <c r="B234" s="3">
-        <v>2025082152</v>
+        <v>2025081053</v>
       </c>
       <c r="C234" s="3">
         <v>1</v>
@@ -18369,16 +18394,16 @@
         <v>632</v>
       </c>
       <c r="F234" s="3" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="G234" s="3" t="s">
-        <v>240</v>
+        <v>687</v>
       </c>
       <c r="H234" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="I234" s="3" t="s">
         <v>689</v>
-      </c>
-      <c r="I234" s="3" t="s">
-        <v>684</v>
       </c>
       <c r="J234" s="3"/>
       <c r="K234" s="3"/>
@@ -18386,10 +18411,10 @@
         <v>145</v>
       </c>
       <c r="M234" s="6" t="s">
-        <v>685</v>
+        <v>690</v>
       </c>
       <c r="N234" s="6" t="s">
-        <v>686</v>
+        <v>691</v>
       </c>
       <c r="O234" s="3" t="s">
         <v>54</v>
@@ -18409,21 +18434,19 @@
         <v>40</v>
       </c>
       <c r="Z234" s="6" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="AA234" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AB234" s="3">
-        <v>1</v>
-      </c>
+      <c r="AB234" s="3"/>
     </row>
     <row r="235" spans="1:28">
       <c r="A235" s="7">
         <v>233</v>
       </c>
       <c r="B235" s="7">
-        <v>2025081606</v>
+        <v>2025082152</v>
       </c>
       <c r="C235" s="7">
         <v>1</v>
@@ -18435,34 +18458,30 @@
         <v>632</v>
       </c>
       <c r="F235" s="7" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="G235" s="7" t="s">
-        <v>199</v>
+        <v>240</v>
       </c>
       <c r="H235" s="7" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="I235" s="7" t="s">
-        <v>692</v>
-      </c>
-      <c r="J235" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="K235" s="7" t="s">
-        <v>144</v>
-      </c>
+        <v>689</v>
+      </c>
+      <c r="J235" s="7"/>
+      <c r="K235" s="7"/>
       <c r="L235" s="8" t="s">
         <v>145</v>
       </c>
       <c r="M235" s="8" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="N235" s="8" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="O235" s="7" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="P235" s="7"/>
       <c r="Q235" s="7"/>
@@ -18475,7 +18494,9 @@
       <c r="V235" s="7"/>
       <c r="W235" s="7"/>
       <c r="X235" s="7"/>
-      <c r="Y235" s="7"/>
+      <c r="Y235" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="Z235" s="8" t="s">
         <v>695</v>
       </c>
@@ -18491,7 +18512,7 @@
         <v>234</v>
       </c>
       <c r="B236" s="3">
-        <v>2025081702</v>
+        <v>2025081606</v>
       </c>
       <c r="C236" s="3">
         <v>1</v>
@@ -18509,10 +18530,10 @@
         <v>199</v>
       </c>
       <c r="H236" s="3" t="s">
-        <v>691</v>
+        <v>696</v>
       </c>
       <c r="I236" s="3" t="s">
-        <v>692</v>
+        <v>697</v>
       </c>
       <c r="J236" s="3" t="s">
         <v>143</v>
@@ -18524,10 +18545,10 @@
         <v>145</v>
       </c>
       <c r="M236" s="6" t="s">
-        <v>693</v>
+        <v>698</v>
       </c>
       <c r="N236" s="6" t="s">
-        <v>694</v>
+        <v>699</v>
       </c>
       <c r="O236" s="3" t="s">
         <v>125</v>
@@ -18545,45 +18566,113 @@
       <c r="X236" s="3"/>
       <c r="Y236" s="3"/>
       <c r="Z236" s="6" t="s">
+        <v>700</v>
+      </c>
+      <c r="AA236" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB236" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:28">
+      <c r="A237" s="7">
+        <v>235</v>
+      </c>
+      <c r="B237" s="7">
+        <v>2025081702</v>
+      </c>
+      <c r="C237" s="7">
+        <v>1</v>
+      </c>
+      <c r="D237" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E237" s="7" t="s">
+        <v>632</v>
+      </c>
+      <c r="F237" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G237" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="H237" s="7" t="s">
         <v>696</v>
       </c>
-      <c r="AA236" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB236" s="3"/>
-    </row>
-    <row r="237" spans="1:28">
-      <c r="A237" s="9"/>
-      <c r="B237" s="9"/>
-      <c r="C237" s="9"/>
-      <c r="D237" s="9"/>
-      <c r="E237" s="9"/>
-      <c r="F237" s="9"/>
-      <c r="G237" s="9"/>
-      <c r="H237" s="9"/>
-      <c r="I237" s="9"/>
-      <c r="J237" s="9"/>
-      <c r="K237" s="9"/>
-      <c r="L237" s="10"/>
-      <c r="M237" s="10"/>
-      <c r="N237" s="10"/>
-      <c r="O237" s="9"/>
-      <c r="P237" s="9"/>
-      <c r="Q237" s="9"/>
-      <c r="R237" s="9"/>
-      <c r="S237" s="9"/>
-      <c r="T237" s="9"/>
-      <c r="U237" s="9"/>
-      <c r="V237" s="9"/>
-      <c r="W237" s="9"/>
-      <c r="X237" s="9"/>
-      <c r="Y237" s="9"/>
-      <c r="Z237" s="10"/>
-      <c r="AA237" s="9" t="s">
+      <c r="I237" s="7" t="s">
         <v>697</v>
       </c>
-      <c r="AB237" s="9">
-        <v>140</v>
+      <c r="J237" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="K237" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="L237" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="M237" s="8" t="s">
+        <v>698</v>
+      </c>
+      <c r="N237" s="8" t="s">
+        <v>699</v>
+      </c>
+      <c r="O237" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="P237" s="7"/>
+      <c r="Q237" s="7"/>
+      <c r="R237" s="7">
+        <v>0</v>
+      </c>
+      <c r="S237" s="7"/>
+      <c r="T237" s="7"/>
+      <c r="U237" s="7"/>
+      <c r="V237" s="7"/>
+      <c r="W237" s="7"/>
+      <c r="X237" s="7"/>
+      <c r="Y237" s="7"/>
+      <c r="Z237" s="8" t="s">
+        <v>701</v>
+      </c>
+      <c r="AA237" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB237" s="7"/>
+    </row>
+    <row r="238" spans="1:28">
+      <c r="A238" s="9"/>
+      <c r="B238" s="9"/>
+      <c r="C238" s="9"/>
+      <c r="D238" s="9"/>
+      <c r="E238" s="9"/>
+      <c r="F238" s="9"/>
+      <c r="G238" s="9"/>
+      <c r="H238" s="9"/>
+      <c r="I238" s="9"/>
+      <c r="J238" s="9"/>
+      <c r="K238" s="9"/>
+      <c r="L238" s="10"/>
+      <c r="M238" s="10"/>
+      <c r="N238" s="10"/>
+      <c r="O238" s="9"/>
+      <c r="P238" s="9"/>
+      <c r="Q238" s="9"/>
+      <c r="R238" s="9"/>
+      <c r="S238" s="9"/>
+      <c r="T238" s="9"/>
+      <c r="U238" s="9"/>
+      <c r="V238" s="9"/>
+      <c r="W238" s="9"/>
+      <c r="X238" s="9"/>
+      <c r="Y238" s="9"/>
+      <c r="Z238" s="10"/>
+      <c r="AA238" s="9" t="s">
+        <v>702</v>
+      </c>
+      <c r="AB238" s="9">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>